<commit_message>
Add MLCLSP model data validation checks
</commit_message>
<xml_diff>
--- a/szablony/MLCLSP_wejscie.xlsx
+++ b/szablony/MLCLSP_wejscie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\STUDIA\MAGISTERKA\Python\WPy64-3771\notebooks\magisterka\mock_input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\STUDIA\MAGISTERKA\Python\WPy64-3771\notebooks\magisterka\szablony\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B64347-92EB-4CC3-A927-DCD9CE1AD7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1841739D-4BF8-4846-9E50-E7B5C542CE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WYROBY" sheetId="2" r:id="rId1"/>
@@ -521,9 +521,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -540,7 +540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -557,7 +557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -574,7 +574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -591,7 +591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -621,9 +621,9 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -634,7 +634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -645,7 +645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -656,7 +656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -667,7 +667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -692,9 +692,9 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -711,7 +711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -728,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -745,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -762,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -793,9 +793,9 @@
       <selection activeCell="F19" sqref="F19:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -809,7 +809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -823,7 +823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -851,7 +851,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -875,11 +875,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F799A6C2-5E4D-434D-A9EE-3D27429D4330}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -893,7 +895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -907,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -921,7 +923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -935,7 +937,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -959,13 +961,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F0377FE-39D8-41BB-9DD0-FBBF85BD9602}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -976,7 +978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -987,7 +989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -998,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>

</xml_diff>